<commit_message>
Adding the selenium search option
</commit_message>
<xml_diff>
--- a/server_input.xlsx
+++ b/server_input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\codes\server_validate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5886B4-E88E-41A6-B2A6-6F527F87CB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CFE3315-7472-4606-869B-3E4228B259F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>url</t>
   </si>
@@ -58,13 +58,19 @@
   </si>
   <si>
     <t>192.168.59.88</t>
+  </si>
+  <si>
+    <t>find text</t>
+  </si>
+  <si>
+    <t>Google </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,6 +91,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3C4043"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -108,9 +120,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -392,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -404,7 +417,7 @@
     <col min="3" max="3" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -414,8 +427,11 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -425,8 +441,11 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -434,7 +453,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -442,12 +461,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -458,5 +477,6 @@
     <hyperlink ref="C2" r:id="rId1" xr:uid="{520AAAE6-78FB-41DE-BBEF-9AD7521ADDAD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>